<commit_message>
Additional Analysis on 800-53
</commit_message>
<xml_diff>
--- a/SP 800-171 Analysis.xlsx
+++ b/SP 800-171 Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juliasmadja/Desktop/GitHub/FedRAMP_SP-800-171_Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A973B81-5AAE-E24D-AA6C-C39141333478}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BC9932-FDAF-EA4A-BF1B-36D8AC123BE7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
     <sheet name="Count_SR_SC" sheetId="11" r:id="rId13"/>
     <sheet name="Names_SR_SC" sheetId="23" r:id="rId14"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -17725,7 +17725,7 @@
   <dimension ref="A1:E201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>